<commit_message>
new gantt chart + new directory for the final checkpoint report images
</commit_message>
<xml_diff>
--- a/ML spring 2025 plan.xlsx
+++ b/ML spring 2025 plan.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3DC3A7-5013-490A-8A24-29E56047F2A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551FF336-CCD2-4FD4-BF40-551F2ED6ACC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,9 +173,6 @@
     <t>Model 1 (Supervised - Logistic Regression): Implementation &amp; Evaluation</t>
   </si>
   <si>
-    <t>Model 2 (Unsupervised - SOM + Classifier): Implementation &amp; Evaluation</t>
-  </si>
-  <si>
     <t>Fairness Adjustment: Adversarial Training to Reduce Bias</t>
   </si>
   <si>
@@ -216,6 +213,9 @@
   </si>
   <si>
     <t>ML Spring 2025 Plan</t>
+  </si>
+  <si>
+    <t>Model 2 (Supervised - Naïve Bayes): Implementation &amp; Evaluation</t>
   </si>
 </sst>
 </file>
@@ -597,7 +597,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -655,6 +655,30 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -684,36 +708,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1174,8 +1168,8 @@
   </sheetPr>
   <dimension ref="B1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1192,7 +1186,7 @@
   <sheetData>
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
       <c r="B1" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -1212,69 +1206,69 @@
         <v>5</v>
       </c>
       <c r="H2" s="11">
+        <v>12</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="28"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="28"/>
+      <c r="AE2" s="28"/>
+      <c r="AF2" s="28"/>
+      <c r="AG2" s="36"/>
       <c r="AH2" s="16"/>
-      <c r="AI2" s="19" t="s">
+      <c r="AI2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="20"/>
+      <c r="AJ2" s="28"/>
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="28"/>
+      <c r="AN2" s="28"/>
+      <c r="AO2" s="28"/>
+      <c r="AP2" s="28"/>
     </row>
     <row r="3" spans="2:67" s="8" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="31" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="17" t="s">
@@ -1302,11 +1296,11 @@
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="29"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1489,508 +1483,508 @@
       </c>
     </row>
     <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="35">
-        <v>1</v>
-      </c>
-      <c r="D5" s="35">
-        <v>2</v>
-      </c>
-      <c r="E5" s="35">
-        <v>1</v>
-      </c>
-      <c r="F5" s="35">
-        <v>2</v>
-      </c>
-      <c r="G5" s="36">
+      <c r="C5" s="23">
+        <v>1</v>
+      </c>
+      <c r="D5" s="23">
+        <v>2</v>
+      </c>
+      <c r="E5" s="23">
+        <v>1</v>
+      </c>
+      <c r="F5" s="23">
+        <v>2</v>
+      </c>
+      <c r="G5" s="24">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:67" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="33">
-        <v>2</v>
-      </c>
-      <c r="D6" s="33">
-        <v>2</v>
-      </c>
-      <c r="E6" s="33">
-        <v>2</v>
-      </c>
-      <c r="F6" s="33">
-        <v>2</v>
-      </c>
-      <c r="G6" s="34">
+      <c r="C6" s="21">
+        <v>2</v>
+      </c>
+      <c r="D6" s="21">
+        <v>2</v>
+      </c>
+      <c r="E6" s="21">
+        <v>2</v>
+      </c>
+      <c r="F6" s="21">
+        <v>2</v>
+      </c>
+      <c r="G6" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="21">
         <v>4</v>
       </c>
-      <c r="D7" s="33">
-        <v>2</v>
-      </c>
-      <c r="E7" s="33">
+      <c r="D7" s="21">
+        <v>2</v>
+      </c>
+      <c r="E7" s="21">
         <v>4</v>
       </c>
-      <c r="F7" s="33">
-        <v>2</v>
-      </c>
-      <c r="G7" s="34">
-        <v>0</v>
+      <c r="F7" s="21">
+        <v>2</v>
+      </c>
+      <c r="G7" s="22">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="21">
         <v>4</v>
       </c>
-      <c r="D8" s="33">
-        <v>2</v>
-      </c>
-      <c r="E8" s="33">
+      <c r="D8" s="21">
+        <v>2</v>
+      </c>
+      <c r="E8" s="21">
         <v>4</v>
       </c>
-      <c r="F8" s="33">
-        <v>2</v>
-      </c>
-      <c r="G8" s="34">
-        <v>0</v>
+      <c r="F8" s="21">
+        <v>2</v>
+      </c>
+      <c r="G8" s="22">
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="21">
         <v>5</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="21">
         <v>3</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="21">
         <v>5</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="21">
         <v>3</v>
       </c>
-      <c r="G9" s="34">
-        <v>0</v>
+      <c r="G9" s="22">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="21">
+        <v>9</v>
+      </c>
+      <c r="D10" s="21">
+        <v>2</v>
+      </c>
+      <c r="E10" s="21">
+        <v>9</v>
+      </c>
+      <c r="F10" s="21">
+        <v>2</v>
+      </c>
+      <c r="G10" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="33">
-        <v>5</v>
-      </c>
-      <c r="D10" s="33">
+      <c r="C11" s="21">
+        <v>8</v>
+      </c>
+      <c r="D11" s="21">
         <v>3</v>
       </c>
-      <c r="E10" s="33">
-        <v>5</v>
-      </c>
-      <c r="F10" s="33">
+      <c r="E11" s="21">
+        <v>8</v>
+      </c>
+      <c r="F11" s="21">
         <v>3</v>
       </c>
-      <c r="G10" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="31" t="s">
+      <c r="G11" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C12" s="21">
+        <v>6</v>
+      </c>
+      <c r="D12" s="21">
+        <v>2</v>
+      </c>
+      <c r="E12" s="21">
+        <v>6</v>
+      </c>
+      <c r="F12" s="21">
+        <v>2</v>
+      </c>
+      <c r="G12" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="21">
         <v>7</v>
       </c>
-      <c r="D11" s="33">
-        <v>3</v>
-      </c>
-      <c r="E11" s="33">
+      <c r="D13" s="21">
+        <v>1</v>
+      </c>
+      <c r="E13" s="21">
         <v>7</v>
       </c>
-      <c r="F11" s="33">
-        <v>3</v>
-      </c>
-      <c r="G11" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="33">
-        <v>6</v>
-      </c>
-      <c r="D12" s="33">
-        <v>2</v>
-      </c>
-      <c r="E12" s="33">
-        <v>6</v>
-      </c>
-      <c r="F12" s="33">
-        <v>2</v>
-      </c>
-      <c r="G12" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="31" t="s">
+      <c r="F13" s="21">
+        <v>1</v>
+      </c>
+      <c r="G13" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="33">
-        <v>7</v>
-      </c>
-      <c r="D13" s="33">
-        <v>1</v>
-      </c>
-      <c r="E13" s="33">
-        <v>7</v>
-      </c>
-      <c r="F13" s="33">
-        <v>1</v>
-      </c>
-      <c r="G13" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="31" t="s">
+      <c r="C14" s="21">
+        <v>9</v>
+      </c>
+      <c r="D14" s="21">
+        <v>2</v>
+      </c>
+      <c r="E14" s="21">
+        <v>9</v>
+      </c>
+      <c r="F14" s="21">
+        <v>2</v>
+      </c>
+      <c r="G14" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="33">
-        <v>8</v>
-      </c>
-      <c r="D14" s="33">
-        <v>2</v>
-      </c>
-      <c r="E14" s="33">
-        <v>8</v>
-      </c>
-      <c r="F14" s="33">
-        <v>2</v>
-      </c>
-      <c r="G14" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="31" t="s">
+      <c r="C15" s="21">
+        <v>10</v>
+      </c>
+      <c r="D15" s="21">
+        <v>2</v>
+      </c>
+      <c r="E15" s="21">
+        <v>10</v>
+      </c>
+      <c r="F15" s="21">
+        <v>2</v>
+      </c>
+      <c r="G15" s="22">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="33">
+      <c r="C16" s="21">
+        <v>10</v>
+      </c>
+      <c r="D16" s="21">
+        <v>2</v>
+      </c>
+      <c r="E16" s="21">
+        <v>10</v>
+      </c>
+      <c r="F16" s="21">
+        <v>2</v>
+      </c>
+      <c r="G16" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="21">
         <v>9</v>
       </c>
-      <c r="D15" s="33">
-        <v>2</v>
-      </c>
-      <c r="E15" s="33">
+      <c r="D17" s="21">
+        <v>2</v>
+      </c>
+      <c r="E17" s="21">
         <v>9</v>
       </c>
-      <c r="F15" s="33">
-        <v>2</v>
-      </c>
-      <c r="G15" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="31" t="s">
+      <c r="F17" s="21">
+        <v>2</v>
+      </c>
+      <c r="G17" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="33">
-        <v>9</v>
-      </c>
-      <c r="D16" s="33">
-        <v>2</v>
-      </c>
-      <c r="E16" s="33">
-        <v>9</v>
-      </c>
-      <c r="F16" s="33">
-        <v>2</v>
-      </c>
-      <c r="G16" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="33">
-        <v>9</v>
-      </c>
-      <c r="D17" s="33">
-        <v>2</v>
-      </c>
-      <c r="E17" s="33">
-        <v>9</v>
-      </c>
-      <c r="F17" s="33">
-        <v>2</v>
-      </c>
-      <c r="G17" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="31" t="s">
+      <c r="C18" s="21">
+        <v>10</v>
+      </c>
+      <c r="D18" s="21">
+        <v>2</v>
+      </c>
+      <c r="E18" s="21">
+        <v>10</v>
+      </c>
+      <c r="F18" s="21">
+        <v>2</v>
+      </c>
+      <c r="G18" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="33">
+      <c r="C19" s="21">
         <v>10</v>
       </c>
-      <c r="D18" s="33">
-        <v>2</v>
-      </c>
-      <c r="E18" s="33">
+      <c r="D19" s="21">
+        <v>2</v>
+      </c>
+      <c r="E19" s="21">
         <v>10</v>
       </c>
-      <c r="F18" s="33">
-        <v>2</v>
-      </c>
-      <c r="G18" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="31" t="s">
+      <c r="F19" s="21">
+        <v>2</v>
+      </c>
+      <c r="G19" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="33">
-        <v>10</v>
-      </c>
-      <c r="D19" s="33">
-        <v>2</v>
-      </c>
-      <c r="E19" s="33">
-        <v>10</v>
-      </c>
-      <c r="F19" s="33">
-        <v>2</v>
-      </c>
-      <c r="G19" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="31" t="s">
+      <c r="C20" s="21">
+        <v>11</v>
+      </c>
+      <c r="D20" s="21">
+        <v>2</v>
+      </c>
+      <c r="E20" s="21">
+        <v>11</v>
+      </c>
+      <c r="F20" s="21">
+        <v>2</v>
+      </c>
+      <c r="G20" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="33">
+      <c r="C21" s="21">
+        <v>12</v>
+      </c>
+      <c r="D21" s="21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="21">
+        <v>12</v>
+      </c>
+      <c r="F21" s="21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="21">
+        <v>12</v>
+      </c>
+      <c r="D22" s="21">
+        <v>1</v>
+      </c>
+      <c r="E22" s="21">
+        <v>12</v>
+      </c>
+      <c r="F22" s="21">
+        <v>1</v>
+      </c>
+      <c r="G22" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="21">
         <v>11</v>
       </c>
-      <c r="D20" s="33">
-        <v>2</v>
-      </c>
-      <c r="E20" s="33">
+      <c r="D23" s="21">
+        <v>2</v>
+      </c>
+      <c r="E23" s="21">
         <v>11</v>
       </c>
-      <c r="F20" s="33">
-        <v>2</v>
-      </c>
-      <c r="G20" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="33">
-        <v>11</v>
-      </c>
-      <c r="D21" s="33">
-        <v>2</v>
-      </c>
-      <c r="E21" s="33">
-        <v>11</v>
-      </c>
-      <c r="F21" s="33">
-        <v>2</v>
-      </c>
-      <c r="G21" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="33">
-        <v>12</v>
-      </c>
-      <c r="D22" s="33">
-        <v>1</v>
-      </c>
-      <c r="E22" s="33">
-        <v>12</v>
-      </c>
-      <c r="F22" s="33">
-        <v>1</v>
-      </c>
-      <c r="G22" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="33">
-        <v>12</v>
-      </c>
-      <c r="D23" s="33">
-        <v>1</v>
-      </c>
-      <c r="E23" s="33">
-        <v>12</v>
-      </c>
-      <c r="F23" s="33">
-        <v>1</v>
-      </c>
-      <c r="G23" s="34">
-        <v>0</v>
+      <c r="F23" s="21">
+        <v>2</v>
+      </c>
+      <c r="G23" s="22">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="31"/>
-      <c r="C24" s="38">
-        <v>0</v>
-      </c>
-      <c r="D24" s="33">
-        <v>0</v>
-      </c>
-      <c r="E24" s="33">
-        <v>0</v>
-      </c>
-      <c r="F24" s="33">
-        <v>0</v>
-      </c>
-      <c r="G24" s="34">
+      <c r="B24" s="20"/>
+      <c r="C24" s="26">
+        <v>0</v>
+      </c>
+      <c r="D24" s="21">
+        <v>0</v>
+      </c>
+      <c r="E24" s="21">
+        <v>0</v>
+      </c>
+      <c r="F24" s="21">
+        <v>0</v>
+      </c>
+      <c r="G24" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="31"/>
-      <c r="C25" s="38">
-        <v>0</v>
-      </c>
-      <c r="D25" s="33">
-        <v>0</v>
-      </c>
-      <c r="E25" s="33">
-        <v>0</v>
-      </c>
-      <c r="F25" s="33">
-        <v>0</v>
-      </c>
-      <c r="G25" s="34">
+      <c r="B25" s="20"/>
+      <c r="C25" s="26">
+        <v>0</v>
+      </c>
+      <c r="D25" s="21">
+        <v>0</v>
+      </c>
+      <c r="E25" s="21">
+        <v>0</v>
+      </c>
+      <c r="F25" s="21">
+        <v>0</v>
+      </c>
+      <c r="G25" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="31"/>
-      <c r="C26" s="38">
-        <v>0</v>
-      </c>
-      <c r="D26" s="33">
-        <v>0</v>
-      </c>
-      <c r="E26" s="33">
-        <v>0</v>
-      </c>
-      <c r="F26" s="33">
-        <v>0</v>
-      </c>
-      <c r="G26" s="34">
+      <c r="B26" s="20"/>
+      <c r="C26" s="26">
+        <v>0</v>
+      </c>
+      <c r="D26" s="21">
+        <v>0</v>
+      </c>
+      <c r="E26" s="21">
+        <v>0</v>
+      </c>
+      <c r="F26" s="21">
+        <v>0</v>
+      </c>
+      <c r="G26" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="31"/>
-      <c r="C27" s="38">
-        <v>0</v>
-      </c>
-      <c r="D27" s="33">
-        <v>0</v>
-      </c>
-      <c r="E27" s="33">
-        <v>0</v>
-      </c>
-      <c r="F27" s="33">
-        <v>0</v>
-      </c>
-      <c r="G27" s="34">
+      <c r="B27" s="20"/>
+      <c r="C27" s="26">
+        <v>0</v>
+      </c>
+      <c r="D27" s="21">
+        <v>0</v>
+      </c>
+      <c r="E27" s="21">
+        <v>0</v>
+      </c>
+      <c r="F27" s="21">
+        <v>0</v>
+      </c>
+      <c r="G27" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="31"/>
-      <c r="C28" s="38">
-        <v>0</v>
-      </c>
-      <c r="D28" s="33">
-        <v>0</v>
-      </c>
-      <c r="E28" s="33">
-        <v>0</v>
-      </c>
-      <c r="F28" s="33">
-        <v>0</v>
-      </c>
-      <c r="G28" s="34">
+      <c r="B28" s="20"/>
+      <c r="C28" s="26">
+        <v>0</v>
+      </c>
+      <c r="D28" s="21">
+        <v>0</v>
+      </c>
+      <c r="E28" s="21">
+        <v>0</v>
+      </c>
+      <c r="F28" s="21">
+        <v>0</v>
+      </c>
+      <c r="G28" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="31"/>
-      <c r="C29" s="38">
-        <v>0</v>
-      </c>
-      <c r="D29" s="33">
-        <v>0</v>
-      </c>
-      <c r="E29" s="33">
-        <v>0</v>
-      </c>
-      <c r="F29" s="33">
-        <v>0</v>
-      </c>
-      <c r="G29" s="34">
+      <c r="B29" s="20"/>
+      <c r="C29" s="26">
+        <v>0</v>
+      </c>
+      <c r="D29" s="21">
+        <v>0</v>
+      </c>
+      <c r="E29" s="21">
+        <v>0</v>
+      </c>
+      <c r="F29" s="21">
+        <v>0</v>
+      </c>
+      <c r="G29" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="31"/>
-      <c r="C30" s="38">
-        <v>0</v>
-      </c>
-      <c r="D30" s="33">
-        <v>0</v>
-      </c>
-      <c r="E30" s="33">
-        <v>0</v>
-      </c>
-      <c r="F30" s="33">
-        <v>0</v>
-      </c>
-      <c r="G30" s="34">
+      <c r="B30" s="20"/>
+      <c r="C30" s="26">
+        <v>0</v>
+      </c>
+      <c r="D30" s="21">
+        <v>0</v>
+      </c>
+      <c r="E30" s="21">
+        <v>0</v>
+      </c>
+      <c r="F30" s="21">
+        <v>0</v>
+      </c>
+      <c r="G30" s="22">
         <v>0</v>
       </c>
     </row>

</xml_diff>